<commit_message>
New Era: League Expansion
</commit_message>
<xml_diff>
--- a/Input/Leagues 22-to-21.xlsx
+++ b/Input/Leagues 22-to-21.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\Coding\GitHub Repos\eFootball-Database-Scrapper\Teams &amp; Competitions\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\OneDrive\Documents\GitHub\PES-Master-CompsAndTeam-Grabber\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F41DCD-2E94-4635-97AC-ACE7CF2E2E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB8EEF4-30B6-4DF8-A8E1-DDEBB138EB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20460" windowHeight="10770" xr2:uid="{269B7300-8F4F-443E-A8C4-E0FEB8C2F215}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{269B7300-8F4F-443E-A8C4-E0FEB8C2F215}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Leagues_22_to_21" localSheetId="0">Sheet1!$A$1:$H$32</definedName>
+    <definedName name="Leagues_22_to_21" localSheetId="0">Sheet1!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>name21</t>
   </si>
@@ -138,18 +137,12 @@
     <t>Ligue 2 BKT</t>
   </si>
   <si>
-    <t>J1 League</t>
-  </si>
-  <si>
     <t>English 2nd Division</t>
   </si>
   <si>
     <t>Championship</t>
   </si>
   <si>
-    <t>J2 League</t>
-  </si>
-  <si>
     <t>English League</t>
   </si>
   <si>
@@ -210,9 +203,6 @@
     <t>Other Teams (Latin America)</t>
   </si>
   <si>
-    <t>PLA League</t>
-  </si>
-  <si>
     <t>MLS</t>
   </si>
   <si>
@@ -241,9 +231,6 @@
   </si>
   <si>
     <t>La Liga</t>
-  </si>
-  <si>
-    <t>Spor Toto Sâ”œâ•per Lig</t>
   </si>
   <si>
     <t>Superliga Quilmes Clâ”œÄªsica</t>
@@ -632,29 +619,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8B23DE-8550-40A3-81B8-DC7A34E7DE9E}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,22 +657,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -692,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -705,24 +694,6 @@
       <c r="D2">
         <v>549</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>635</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>269</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2">
-        <v>476</v>
-      </c>
       <c r="K2" t="s">
         <v>7</v>
       </c>
@@ -730,7 +701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -743,12 +714,6 @@
       <c r="D3">
         <v>101</v>
       </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3">
-        <v>603</v>
-      </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
@@ -756,7 +721,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -776,7 +741,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -796,7 +761,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -816,7 +781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -836,7 +801,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -850,344 +815,370 @@
         <v>343</v>
       </c>
       <c r="K8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>27</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
       </c>
       <c r="B9">
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>337</v>
       </c>
-      <c r="K9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>113</v>
       </c>
-      <c r="K10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="D12">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
       <c r="B13">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
       </c>
       <c r="D15">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="D16">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B17">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B18">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>45</v>
-      </c>
-      <c r="B19">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>46</v>
       </c>
       <c r="B20">
         <v>34</v>
       </c>
       <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
       <c r="B21">
-        <v>34</v>
+        <v>204</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
       <c r="D21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="B22">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
       <c r="B23">
-        <v>212</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D24">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>54</v>
       </c>
       <c r="D25">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
         <v>56</v>
       </c>
       <c r="D26">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
       <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>131</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
         <v>69</v>
       </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28">
-        <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31">
-        <v>139</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31">
-        <v>585</v>
+      <c r="D35">
+        <v>476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>